<commit_message>
Contains Initial Data for my Inventory
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koner\Desktop\Git_repo\ETG-Inventory-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780B1007-CE9B-4BB9-B2AF-4BC23AC83996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93BB827-AA49-43F1-B5FC-8DA7BBE6AA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2439403F-B582-4C5A-81A9-6410E3C801E9}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{2439403F-B582-4C5A-81A9-6410E3C801E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1353,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B21573C-B18F-462D-9FCD-D48F1568CFE3}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>